<commit_message>
equipos de lab-cesar cargados para test
</commit_message>
<xml_diff>
--- a/equipos.xlsx
+++ b/equipos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csalva\Documents\Cesar\Hello world\NeMikroPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D2C4D7-28F7-436D-8601-FA6B60989D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410863EA-2FF2-44EF-8C19-809271DDB067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39795" yWindow="-2235" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>Router1</t>
-  </si>
-  <si>
-    <t>Switch1</t>
-  </si>
-  <si>
-    <t>192.168.240.134</t>
-  </si>
-  <si>
-    <t>192.168.240.133</t>
-  </si>
-  <si>
     <t>Puerto API</t>
   </si>
   <si>
@@ -49,7 +37,31 @@
     <t>Nombre del Equipo</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>192.168.240.135</t>
+  </si>
+  <si>
+    <t>10.20.0.1</t>
+  </si>
+  <si>
+    <t>10.30.0.2</t>
+  </si>
+  <si>
+    <t>10.50.0.2</t>
+  </si>
+  <si>
+    <t>10.60.0.2</t>
+  </si>
+  <si>
+    <t>172.20.0.2</t>
+  </si>
+  <si>
+    <t>172.30.0.2</t>
+  </si>
+  <si>
+    <t>172.40.0.2</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -452,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,57 +479,132 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>8728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>8728</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>8728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>8728</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>4444</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>4444</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6"/>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>8728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>8728</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>8728</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>8728</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>